<commit_message>
Update WCAG Comparison todo it on Sunday..xlsx
</commit_message>
<xml_diff>
--- a/WCAG Comparison todo it on Sunday..xlsx
+++ b/WCAG Comparison todo it on Sunday..xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derwin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CrimsonHearts\Documents\GitHub\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F6A230-160F-40CA-8D1D-20248001B355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="3170" windowWidth="14400" windowHeight="7360" xr2:uid="{890185DE-B281-4ECA-B2C3-A01216CAB0EE}"/>
+    <workbookView xWindow="11940" yWindow="3165" windowWidth="14400" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>WCAG 1.0</t>
   </si>
@@ -56,16 +55,122 @@
   </si>
   <si>
     <t>Text equivalent for an</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Guidline Organization</t>
+  </si>
+  <si>
+    <t>- The guidline number
+- The Statement of the guideline.
+- Guideline navigation links. Three links allow navigation to the next guideline (right arrow icon), the previous guideline (left arrow icon), the current guideline's position in the table of contents (up arrow icon).
+The rationale behind the guideline and some groups of users who benefit from it.
+A list of checkpoint definition</t>
+  </si>
+  <si>
+    <t>Checkpoint Definition</t>
+  </si>
+  <si>
+    <t>- The checkpoint number
+-  The statement of the checkpoint.
+- Thepriority of the checkpoint. Priority 1 checkpoints are highlighted through the use of style sheets.
+- Optional informative notes, clarifying examples, and cross references to related guidelines or checkpoints
+- A link to a section of the Techniques Document  where implementations and examples of the checkpoint are discussed.</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Each Checkpoint has a priority level assigned by the Working group based on the checkpoint's impact on accessibility.
+One or more groups will find it impossible to access information in the document, if any of the 3 priority are not satisfied.
+[Priority 1]
+A Web content developer must satisfy this checkpoint.  Satisfying this checkpoint is a basic requirement for some groups to be able to use Web documents.
+[Priority 2]
+A Web content developer should satisfy this checkpoint. Satisfying this checkpoitn will remove significant barriers to accessing Web Document
+[Priority3]
+A Web content developer may address this checkpoint. Satisfying this checkpoint will improved access to Web Document</t>
+  </si>
+  <si>
+    <t>Web Content Accessibility Guideline</t>
+  </si>
+  <si>
+    <t>Guidline 1 
+Text Equivalent or Alternative to auditory and visual content</t>
+  </si>
+  <si>
+    <t>Guideline Links:</t>
+  </si>
+  <si>
+    <t>Provide equivalent alternatives to auditory and visual content.
+This specific guideline covers a range where images,videos, text, sounds alternative are important as it's users who have sensory disability or even reading difficulty. However, just implementation of this specific guideline maynot be enough as the text equivalent/alternative may be a good approach to allow accessibility concepts of color/ font size/ font thickness / number of flashes can also be another alternative to further aid it's users to understand the content .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 Provide a text quivalent for every non-text element. </t>
+  </si>
+  <si>
+    <t>This includes: images, graphical representations of text (including symbols), image map regions, animation, applets and programmatic objects, ascii art, frames, scripts, images used as list bullets, spacers, graphical buttons, sounds (played with or without user interaction), stand-alone audio files, audio tracks of video and video.
+Online advertisement in Website/games are one of the areas that may prove to be diffcult in apply text equivalent as Site such youtube where they show dynamicity of advertisement.</t>
+  </si>
+  <si>
+    <t>1.2 Provide redundant text links for each active region of a server-side image map.</t>
+  </si>
+  <si>
+    <t>Providing such text links for each active region of a server-side image map may prove to be a challenge to as some site image are usually redirected to a specific page.
+However using this set of guideline could be useful and implemented across education and health to help provide useful information to allow it's users to have a better understanding of such images.</t>
+  </si>
+  <si>
+    <t>1.3 Until user agents can automatically read aloud the text equivalent of a visual track, provide an auditory description of the important information of the visual track of a multimedia presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to
+- Checkpoint 9.1
+- Checkpoint 13.10
+Techniques:
+https://www.w3.org/TR/WAI-WEBCONTENT-TECHS/#tech-text-equivalent
+Refered Link:
+http://dsq-sds.org/article/view/281/311
+</t>
+  </si>
+  <si>
+    <t>Refer to:
+- Checkpoint 1.5
+- Checkpoint 9.1
+Techniques:
+https://www.w3.org/TR/WAI-WEBCONTENT-TECHS/#tech-redundant-server-links</t>
+  </si>
+  <si>
+    <t>Refer to:
+- Checkpoint 1.4
+- Checkpoint 1.1
+Techniques: 
+http://www.w3.org/TR/WAI-WEBCONTENT-TECHS/#tech-auditory-descriptions</t>
+  </si>
+  <si>
+    <t>More research on the range and variety of user agent compatibility is required.
+However, in the event where the user agents are unable to provide it's user with proper information</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WAI-WEBCONTENT/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,19 +193,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,54 +520,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6CA721-92B8-4941-A5E1-8820B2E43367}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="288" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="116" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>